<commit_message>
changes in ExcelUtils class
</commit_message>
<xml_diff>
--- a/excel-output/Hotel Details.xlsx
+++ b/excel-output/Hotel Details.xlsx
@@ -29,28 +29,28 @@
     <t>Holiday Inn NAIROBI TWO RIVERS MALL by IHG</t>
   </si>
   <si>
-    <t>₹ 22,207</t>
+    <t>₹ 21,063</t>
   </si>
   <si>
-    <t>₹ 142,125</t>
+    <t>₹ 134,802</t>
   </si>
   <si>
     <t>JW Marriott Hotel Nairobi</t>
   </si>
   <si>
-    <t>₹ 207,571</t>
+    <t>₹ 206,210</t>
   </si>
   <si>
-    <t>₹ 1,310,397</t>
+    <t>₹ 1,301,801</t>
   </si>
   <si>
     <t>Yaya Hotel &amp; Apartments</t>
   </si>
   <si>
-    <t>₹ 19,982</t>
+    <t>₹ 19,945</t>
   </si>
   <si>
-    <t>₹ 98,836</t>
+    <t>₹ 96,167</t>
   </si>
 </sst>
 </file>

</xml_diff>